<commit_message>
Agrega piers ejes 6, 11, 13
</commit_message>
<xml_diff>
--- a/Tarea 06/muros.xlsx
+++ b/Tarea 06/muros.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E4AAFFD5-3CDF-4FE2-A51D-A8A256486D34}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{64C3FF80-D58D-4092-90DA-765888C990BE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="85">
   <si>
     <t>As [cm2/m]</t>
   </si>
@@ -149,9 +149,6 @@
     <t>Separación (s)</t>
   </si>
   <si>
-    <t>Vs total</t>
-  </si>
-  <si>
     <t>Resistencia total sin reducir</t>
   </si>
   <si>
@@ -170,9 +167,6 @@
     <t>Corte resistente total</t>
   </si>
   <si>
-    <t>Vn max</t>
-  </si>
-  <si>
     <t>[-]</t>
   </si>
   <si>
@@ -215,18 +209,12 @@
     <t>Largo del muro ($l_w$)</t>
   </si>
   <si>
-    <t>Real</t>
-  </si>
-  <si>
     <t>${Vc}_1$</t>
   </si>
   <si>
     <t>Cuantía requerida</t>
   </si>
   <si>
-    <t>Resistencia acero con el acero definido</t>
-  </si>
-  <si>
     <t>Área de una barra</t>
   </si>
   <si>
@@ -279,6 +267,15 @@
   </si>
   <si>
     <t>Vn FINAL</t>
+  </si>
+  <si>
+    <t>Sin redondear</t>
+  </si>
+  <si>
+    <t>Vs FINAL</t>
+  </si>
+  <si>
+    <t>Resistencia acero con el acero definido, limitada por Vs max</t>
   </si>
 </sst>
 </file>
@@ -879,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -901,7 +898,7 @@
         <v>18</v>
       </c>
       <c r="K2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -921,7 +918,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L3">
         <v>350</v>
@@ -948,7 +945,7 @@
         <v>1.0666666666666667</v>
       </c>
       <c r="K4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L4">
         <v>300</v>
@@ -975,7 +972,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="K5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1710,10 +1707,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ACFD7F1-EE11-4176-B28A-840FC552FF55}">
-  <dimension ref="B2:Q59"/>
+  <dimension ref="B2:Q57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1730,6 +1727,7 @@
     <col min="10" max="10" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="1.88671875" customWidth="1"/>
     <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1757,11 +1755,11 @@
         <v>7</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I5" s="16">
         <f>C12/16</f>
-        <v>937.5</v>
+        <v>15.625</v>
       </c>
       <c r="J5" s="16" t="s">
         <v>4</v>
@@ -1769,7 +1767,7 @@
       <c r="K5" s="21"/>
       <c r="L5" s="38" t="str">
         <f>IF(I5&lt;C10,"[OK]","[REDISEÑAR]")</f>
-        <v>[REDISEÑAR]</v>
+        <v>[OK]</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
@@ -1805,7 +1803,7 @@
         <v>7</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I7" s="16">
         <f>MIN(0.8*C11/5,3*C10,45)</f>
@@ -1822,7 +1820,7 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H8" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I8" s="16">
         <f>MIN(0.8*C12/3,3*C11,45)</f>
@@ -1842,7 +1840,7 @@
         <v>3</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I9" s="16">
         <f>0.8*C11</f>
@@ -1866,7 +1864,7 @@
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C11" s="16">
         <v>500</v>
@@ -1883,7 +1881,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="16">
-        <v>15000</v>
+        <v>250</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>4</v>
@@ -1934,7 +1932,7 @@
         <v>11</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
@@ -1948,7 +1946,7 @@
         <v>11</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I16" s="16">
         <f>1.2*C16+C17+1.4*C18</f>
@@ -1958,7 +1956,7 @@
         <v>11</v>
       </c>
       <c r="L16" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
@@ -1972,7 +1970,7 @@
         <v>11</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I17" s="16">
         <f>SUM(C16:C18)</f>
@@ -1982,7 +1980,7 @@
         <v>11</v>
       </c>
       <c r="L17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.3">
@@ -1996,7 +1994,7 @@
         <v>11</v>
       </c>
       <c r="H18" s="19" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I18" s="16">
         <f>IF(C19=0,I16,C19)</f>
@@ -2006,12 +2004,12 @@
         <v>11</v>
       </c>
       <c r="L18" s="39" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B19" s="19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C19" s="16">
         <v>150</v>
@@ -2020,7 +2018,7 @@
         <v>11</v>
       </c>
       <c r="H19" s="19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I19" s="16">
         <f>IF(C19=0,I17,C19)</f>
@@ -2030,7 +2028,7 @@
         <v>11</v>
       </c>
       <c r="L19" s="39" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
@@ -2038,7 +2036,7 @@
         <v>40</v>
       </c>
       <c r="H21" s="26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
@@ -2077,7 +2075,7 @@
         <v>[OK]</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I23" s="29">
         <f>MAX(I22*100*C10/(2*C7),C27)</f>
@@ -2107,7 +2105,7 @@
         <v>[OK</v>
       </c>
       <c r="M24" s="40" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="N24" s="41">
         <f>1/I23*(C22/2)^2*PI()</f>
@@ -2120,10 +2118,10 @@
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B25" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H25" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I25" s="29">
         <f>C26*2*IF(C11/C23&gt;=1,C11/C23,0)</f>
@@ -2137,7 +2135,7 @@
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B26" s="30" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C26" s="29">
         <f>(C22/(2*10))^2*PI()</f>
@@ -2147,7 +2145,7 @@
         <v>16</v>
       </c>
       <c r="H26" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I26" s="33">
         <f>C7*I25/1000</f>
@@ -2171,7 +2169,7 @@
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B27" s="30" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C27" s="29">
         <f>2.5/1000*100*C10/2</f>
@@ -2184,10 +2182,10 @@
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.3">
       <c r="H28" s="18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L28" s="17" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.3">
@@ -2198,10 +2196,10 @@
         <v>0.6</v>
       </c>
       <c r="J29" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L29" s="19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="M29" s="29">
         <f>SQRT(C5*0.0980665)*(1/0.0980665)/1000*I31*0.17</f>
@@ -2213,7 +2211,7 @@
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.3">
       <c r="H30" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I30" s="33">
         <f>I18/I29</f>
@@ -2223,14 +2221,14 @@
         <v>11</v>
       </c>
       <c r="L30" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M30" s="16">
         <f>IF(C12/I9&lt;=1.5,0.25,IF(C12/I9&gt;=2,0.17,0.17+(0.25-0.17)/(C12/I9-1.5)*C12/I9))</f>
-        <v>0.17</v>
+        <v>0.25</v>
       </c>
       <c r="N30" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.3">
@@ -2245,11 +2243,11 @@
         <v>16</v>
       </c>
       <c r="L31" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M31" s="29">
         <f>SQRT(C5*0.0980665)*(1/0.0980665)/1000*I31*M30</f>
-        <v>74.799027579460727</v>
+        <v>109.99856996979518</v>
       </c>
       <c r="N31" s="28" t="s">
         <v>11</v>
@@ -2257,7 +2255,7 @@
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.3">
       <c r="H32" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I32" s="33">
         <f>MIN(M31,M29)</f>
@@ -2281,7 +2279,7 @@
     </row>
     <row r="34" spans="8:17" x14ac:dyDescent="0.3">
       <c r="H34" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I34" s="36">
         <f>MAX(I33/(C6*I9/1000/100)/2,C27)</f>
@@ -2293,26 +2291,26 @@
     </row>
     <row r="35" spans="8:17" x14ac:dyDescent="0.3">
       <c r="H35" s="19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I35" s="35">
         <f>I34/C10/100*2</f>
         <v>4.1714517242985539E-3</v>
       </c>
       <c r="J35" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="8:17" x14ac:dyDescent="0.3">
       <c r="H36" s="19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I36" s="16">
         <f>MAX(0.0025,0.0025*0.5*(2.5-C10/(C11*0.8))*(I35-0.0025))</f>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J36" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L36" s="38" t="str">
         <f>IF(OR(I35&gt;I36,ABS(I35-I36)&lt;0.0001),"[OK]","[REDISEÑAR]")</f>
@@ -2322,7 +2320,7 @@
     </row>
     <row r="37" spans="8:17" x14ac:dyDescent="0.3">
       <c r="H37" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I37" s="33">
         <f>SQRT(C5*0.0980665)*(1/0.0980665)/1000*0.66*0.8*C11*C10</f>
@@ -2332,7 +2330,7 @@
         <v>11</v>
       </c>
       <c r="L37" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N37" s="15"/>
     </row>
@@ -2352,7 +2350,7 @@
         <v>[OK</v>
       </c>
       <c r="M38" s="40" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="N38" s="41">
         <f>1/I34*(C22/2)^2*PI()</f>
@@ -2366,7 +2364,7 @@
     </row>
     <row r="39" spans="8:17" x14ac:dyDescent="0.3">
       <c r="H39" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I39" s="29">
         <f>C26*2*IF(I9/C23&gt;=1,I9/C23,0)</f>
@@ -2380,7 +2378,7 @@
     </row>
     <row r="40" spans="8:17" x14ac:dyDescent="0.3">
       <c r="H40" s="19" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="I40" s="33">
         <f>MIN(I39*C6/1000,I37)</f>
@@ -2390,14 +2388,14 @@
         <v>11</v>
       </c>
       <c r="L40" s="39" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="M40" s="15"/>
       <c r="N40" s="15"/>
     </row>
     <row r="41" spans="8:17" x14ac:dyDescent="0.3">
       <c r="H41" s="19" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="I41" s="33">
         <f>I40+I32</f>
@@ -2406,117 +2404,88 @@
       <c r="J41" s="16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="42" spans="8:17" x14ac:dyDescent="0.3">
-      <c r="H42" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="I42" s="33">
-        <f>0.66*SQRT(C5*0.0980665)*(1/0.0980665)/1000*I9*C10</f>
-        <v>365.04316828555454</v>
-      </c>
-      <c r="J42" s="16" t="s">
+      <c r="L41" s="38" t="str">
+        <f>IF(I41&gt;I30,"[OK]","[REDISEÑAR]")</f>
+        <v>[OK]</v>
+      </c>
+      <c r="M41" s="40" t="str">
+        <f>IF(N41&gt;0,"Sobrado","Faltan")</f>
+        <v>Sobrado</v>
+      </c>
+      <c r="N41" s="42">
+        <f>I41-I30</f>
+        <v>13.294586794848328</v>
+      </c>
+    </row>
+    <row r="43" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H43" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="N43" s="15"/>
+    </row>
+    <row r="44" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H44" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="I44" s="16">
+        <f>I18</f>
+        <v>150</v>
+      </c>
+      <c r="J44" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M42" s="15"/>
-      <c r="N42" s="15"/>
-    </row>
-    <row r="43" spans="8:17" x14ac:dyDescent="0.3">
-      <c r="H43" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="I43" s="33">
-        <f>MIN(I42,I41)</f>
-        <v>263.29458679484833</v>
-      </c>
-      <c r="J43" s="16" t="s">
+      <c r="N44" s="25"/>
+    </row>
+    <row r="45" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H45" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="I45" s="33">
+        <f>I30</f>
+        <v>250</v>
+      </c>
+      <c r="J45" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="L43" s="38" t="str">
-        <f>IF(I43&gt;I30,"[OK]","[REDISEÑAR]")</f>
-        <v>[OK]</v>
-      </c>
-      <c r="M43" s="40" t="str">
-        <f>IF(N43&gt;0,"Sobrado","Faltan")</f>
-        <v>Sobrado</v>
-      </c>
-      <c r="N43" s="42">
-        <f>I43-I30</f>
-        <v>13.294586794848328</v>
-      </c>
-    </row>
-    <row r="45" spans="8:17" x14ac:dyDescent="0.3">
-      <c r="H45" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="N45" s="15"/>
     </row>
     <row r="46" spans="8:17" x14ac:dyDescent="0.3">
       <c r="H46" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="I46" s="16">
-        <f>I18</f>
-        <v>150</v>
+        <v>36</v>
+      </c>
+      <c r="I46" s="33">
+        <f>2/3*I31*SQRT(C5*0.0980665)*(1/0.0980665)/1000</f>
+        <v>293.32951991945379</v>
       </c>
       <c r="J46" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="N46" s="25"/>
-    </row>
-    <row r="47" spans="8:17" x14ac:dyDescent="0.3">
-      <c r="H47" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="I47" s="33">
-        <f>I30</f>
-        <v>250</v>
-      </c>
-      <c r="J47" s="16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48" spans="8:17" x14ac:dyDescent="0.3">
-      <c r="H48" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I48" s="33">
-        <f>2/3*I31*SQRT(C5*0.0980665)*(1/0.0980665)/1000</f>
-        <v>293.32951991945379</v>
-      </c>
-      <c r="J48" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="L48" s="38" t="str">
-        <f>IF(I48&gt;I47,"[OK]","[REDISEÑAR]")</f>
+      <c r="L46" s="38" t="str">
+        <f>IF(I46&gt;I45,"[OK]","[REDISEÑAR]")</f>
         <v>[OK]</v>
       </c>
-      <c r="M48" s="40" t="str">
-        <f>IF(N48&gt;0,"Sobrado","Faltan")</f>
+      <c r="M46" s="40" t="str">
+        <f>IF(N46&gt;0,"Sobrado","Faltan")</f>
         <v>Sobrado</v>
       </c>
-      <c r="N48" s="42">
-        <f>I48-I47</f>
+      <c r="N46" s="42">
+        <f>I46-I45</f>
         <v>43.329519919453787</v>
       </c>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H54"/>
+    </row>
+    <row r="55" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H55"/>
     </row>
     <row r="56" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H56"/>
     </row>
     <row r="57" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H57"/>
-    </row>
-    <row r="58" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H58"/>
-    </row>
-    <row r="59" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H59"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="I17" formulaRange="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>